<commit_message>
Modif sur la doc 	modified:   doc/TestValidation.xlsx
</commit_message>
<xml_diff>
--- a/doc/TestValidation.xlsx
+++ b/doc/TestValidation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Situation</t>
   </si>
@@ -74,12 +74,6 @@
     <t>then Res pressed</t>
   </si>
   <si>
-    <t>6a</t>
-  </si>
-  <si>
-    <t>6b</t>
-  </si>
-  <si>
     <t>No effect</t>
   </si>
   <si>
@@ -95,9 +89,6 @@
     <t>Dimunution de X</t>
   </si>
   <si>
-    <t>6c</t>
-  </si>
-  <si>
     <t>Satus INT &amp; Tampomat OFF</t>
   </si>
   <si>
@@ -125,12 +116,6 @@
     <t>Faire le resume</t>
   </si>
   <si>
-    <t xml:space="preserve">controler ON SET OFF et ON </t>
-  </si>
-  <si>
-    <t>j'ai detecter un comportement bizarre</t>
-  </si>
-  <si>
     <t>test les valeur max et min du tampomatt</t>
   </si>
   <si>
@@ -138,9 +123,6 @@
   </si>
   <si>
     <t>retourve last Set value &amp; STATUS ON</t>
-  </si>
-  <si>
-    <t>10a</t>
   </si>
   <si>
     <t xml:space="preserve">Accel &gt;PEDAL_MIN  </t>
@@ -365,14 +347,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -714,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -725,12 +709,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18">
-      <c r="A1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -751,7 +735,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -761,19 +745,19 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -787,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -801,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
@@ -829,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -843,7 +827,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -855,10 +839,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
@@ -869,20 +853,20 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="18">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
@@ -900,55 +884,55 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
-        <v>17</v>
+      <c r="A19" s="4">
+        <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="4" t="s">
-        <v>18</v>
+      <c r="A20" s="4">
+        <v>10</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4">
+        <v>11</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>10</v>
@@ -956,13 +940,13 @@
     </row>
     <row r="22" spans="1:6" ht="20.25" customHeight="1">
       <c r="A22" s="4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>10</v>
@@ -970,13 +954,13 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>10</v>
@@ -984,13 +968,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>10</v>
@@ -998,113 +982,115 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="4">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4">
+        <v>20</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18">
+      <c r="A35" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="8"/>
-      <c r="B30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="18">
-      <c r="A35" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
@@ -1114,57 +1100,65 @@
         <v>0</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="4"/>
+      <c r="A37" s="4">
+        <v>22</v>
+      </c>
       <c r="B37" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="4">
+        <v>23</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="4">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="4">
+        <v>25</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="C40" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1174,7 +1168,6 @@
     <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>